<commit_message>
update coa template angsuran
</commit_message>
<xml_diff>
--- a/public/template-excel/templateuploadangsuran.xlsx
+++ b/public/template-excel/templateuploadangsuran.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DBL IT\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WinNMP\WWW\simpinlaravel\simpin\public\template-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED112F85-6F37-48B3-8004-1AE9DDC5C5C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF2F22B-088A-4712-87DD-17FF280664AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8C1D36D1-47AC-4FA1-BD03-543EE7BF72A5}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>angsuran ke</t>
   </si>
@@ -40,6 +40,12 @@
   </si>
   <si>
     <t>10602060-13782-12032021085512</t>
+  </si>
+  <si>
+    <t>coa</t>
+  </si>
+  <si>
+    <t>102.18.000</t>
   </si>
 </sst>
 </file>
@@ -392,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{055DA7FA-5C58-4747-8D04-84F839402D0E}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -406,7 +412,7 @@
     <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -419,8 +425,11 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -433,8 +442,11 @@
       <c r="D2" s="1">
         <v>44287</v>
       </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -446,6 +458,9 @@
       </c>
       <c r="D3" s="1">
         <v>44287</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>